<commit_message>
Inserts done except 2020,2021,2022
</commit_message>
<xml_diff>
--- a/output/2024-04-07 Postgres insert count.xlsx
+++ b/output/2024-04-07 Postgres insert count.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Greg\Repositories\Lookup-Tables\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32702883-AE33-495F-96C0-061F7AB3AA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C22E9D-3548-4F9F-B6C8-87852AA5194C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{EDD47FC4-FF7D-4012-A995-7DC28037C457}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{EDD47FC4-FF7D-4012-A995-7DC28037C457}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="2024_04_06 run" sheetId="1" r:id="rId5"/>
+    <sheet name="2024_04_08 run" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="16">
   <si>
     <t>fiscal_year</t>
   </si>
@@ -130,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -141,7 +142,6 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,7 +172,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Greg Sanders" refreshedDate="45389.02343645833" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="125" xr:uid="{2B4A5A55-8C3A-49EC-87BC-9A6B97A944E2}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E126" sheet="Sheet1"/>
+    <worksheetSource ref="A1:E126" sheet="2024_04_06 run"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="fiscal_year" numFmtId="0">
@@ -1139,7 +1139,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A262886A-13A5-4952-B0A5-78BF86945031}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A262886A-13A5-4952-B0A5-78BF86945031}" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D165" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -1742,7 +1742,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D52B75DF-F8AC-41D3-A9C4-DB0C58469F2A}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D52B75DF-F8AC-41D3-A9C4-DB0C58469F2A}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C21" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -1911,7 +1911,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C75ADB71-5785-44C9-816F-47DA4FF19491}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C75ADB71-5785-44C9-816F-47DA4FF19491}" name="PivotTable4" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -1976,7 +1976,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2C6755C1-D426-4B59-8E93-ED2CCABDE53F}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2C6755C1-D426-4B59-8E93-ED2CCABDE53F}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -2394,15 +2394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BADF025D-7AA1-4AB3-9F58-99AD0EE6B452}">
   <dimension ref="A3:D165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="A96" activeCellId="33" sqref="A5 A7 A9 A11 A13 A15 A17 A19 A21 A23 A25 A27 A29 A31 A33 A35:A36 A38:A39 A41:A42 A44:A45 A47:A48 A50:A51 A53:A54 A56:A57 A59:A60 A62:A63 A65:A66 A68:A69 A71:A72 A74:A76 A78:A80 A82:A84 A86:A88 A90:A92 A94:A96 A98:A100 A102:A104 A106:A108 A110:A112 A114:A116 A118:A120 A122:A124 A126:A128 A130:A132 A134:A136 A138:A140 A142:A144 A146:A147 A149:A150 A152:A153 A155:A156 A158:A159 A161:A162 A164"/>
-      <pivotSelection pane="bottomRight" showHeader="1" axis="axisRow" dimension="1" activeRow="95" previousRow="95" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-          <references count="1">
-            <reference field="1" count="0"/>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5050,7 +5043,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5">
         <v>230</v>
       </c>
     </row>
@@ -5063,8 +5056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785AF368-6265-44AE-B62E-549F07DE05B2}">
   <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E126"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7214,4 +7207,2025 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{087A450B-56EA-4208-BCCD-B91D41942492}">
+  <dimension ref="A1:E118"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E118"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2006</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>2307757</v>
+      </c>
+      <c r="D2">
+        <v>217568965355.76999</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2012</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2927664</v>
+      </c>
+      <c r="D3">
+        <v>511409029783.34497</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2013</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2276754</v>
+      </c>
+      <c r="D4">
+        <v>453087824485.38202</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>2311888</v>
+      </c>
+      <c r="D5">
+        <v>436516563400.05603</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2020</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5021482</v>
+      </c>
+      <c r="D6">
+        <v>333366978403.80603</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2007</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>1746422</v>
+      </c>
+      <c r="D7">
+        <v>233185499058.33899</v>
+      </c>
+      <c r="E7">
+        <v>233185499061.07001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2011</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>202959</v>
+      </c>
+      <c r="D8">
+        <v>9815112263.5699997</v>
+      </c>
+      <c r="E8">
+        <v>9815112263.5699997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>727431</v>
+      </c>
+      <c r="D9">
+        <v>93321783883.850006</v>
+      </c>
+      <c r="E9">
+        <v>93321783883.850006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>1388484</v>
+      </c>
+      <c r="D10">
+        <v>268287652301.94601</v>
+      </c>
+      <c r="E10">
+        <v>268287664451.82001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2021</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>1175861</v>
+      </c>
+      <c r="D11">
+        <v>307561417612.5</v>
+      </c>
+      <c r="E11">
+        <v>307562279781.47998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2022</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>899115.31980000006</v>
+      </c>
+      <c r="E12">
+        <v>881986.86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1987</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>-171000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1994</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>230094</v>
+      </c>
+      <c r="D14">
+        <v>117964116539</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1970</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>12164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1981</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>1809</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>2736482040.9000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1982</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>1848</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>891945580</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1993</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>2712</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>2934156957</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1997</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>32860</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>27312828123.900002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2002</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>3031221.28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>567750</v>
+      </c>
+      <c r="D21">
+        <v>205302457889.95599</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2003</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>763966</v>
+      </c>
+      <c r="D22">
+        <v>139125853330.78601</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2004</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>1358521</v>
+      </c>
+      <c r="D23">
+        <v>160481119817.258</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2009</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>2252925</v>
+      </c>
+      <c r="D24">
+        <v>281925405610.492</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2017</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>4185509</v>
+      </c>
+      <c r="D25">
+        <v>417317345117.92603</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2003</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>419937</v>
+      </c>
+      <c r="D26">
+        <v>185742657627.17401</v>
+      </c>
+      <c r="E26">
+        <v>185743788104.60999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2006</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>1490396</v>
+      </c>
+      <c r="D27">
+        <v>213448008728.78699</v>
+      </c>
+      <c r="E27">
+        <v>213447362879.69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2009</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>1244572</v>
+      </c>
+      <c r="D28">
+        <v>258888790192.95901</v>
+      </c>
+      <c r="E28">
+        <v>258888790060.82001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2012</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>202205</v>
+      </c>
+      <c r="D29">
+        <v>9359669004.4899998</v>
+      </c>
+      <c r="E29">
+        <v>9359669004.4899998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2014</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>216286</v>
+      </c>
+      <c r="D30">
+        <v>9549372257.8400002</v>
+      </c>
+      <c r="E30">
+        <v>9549372257.8400002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1991</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>249091</v>
+      </c>
+      <c r="D31">
+        <v>136154193844</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1993</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>227903</v>
+      </c>
+      <c r="D32">
+        <v>121373382142</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1997</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>256866</v>
+      </c>
+      <c r="D33">
+        <v>117203970180</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2002</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>1372925.2812999999</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2003</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>3056736</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2011</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>194948</v>
+      </c>
+      <c r="D36">
+        <v>8425313236.6323004</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2015</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>2856181</v>
+      </c>
+      <c r="D37">
+        <v>257359629071.81299</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1985</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>1799</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>1551420893.73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1986</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>1838</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39">
+        <v>1187949278.8499999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1996</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <v>8777</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>4150158274.9099998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2006</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41">
+        <v>6713.69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2020</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42">
+        <v>11105</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42">
+        <v>2467461929.3000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2022</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>11544</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43">
+        <v>1247462476.8199999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2001</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>411732</v>
+      </c>
+      <c r="D44">
+        <v>88847752490.149506</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2002</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>539170</v>
+      </c>
+      <c r="D45">
+        <v>107507962598.67599</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2008</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>2565289</v>
+      </c>
+      <c r="D46">
+        <v>269822179140.09399</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2011</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>3205469</v>
+      </c>
+      <c r="D47">
+        <v>529909130663.95502</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2018</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>4231649</v>
+      </c>
+      <c r="D48">
+        <v>287216989832.93597</v>
+      </c>
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2021</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>5174110</v>
+      </c>
+      <c r="D49">
+        <v>323284502297.966</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2022</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <v>6645255</v>
+      </c>
+      <c r="D50">
+        <v>693388861275.23096</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2002</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51">
+        <v>291462</v>
+      </c>
+      <c r="D51">
+        <v>156513300050.595</v>
+      </c>
+      <c r="E51">
+        <v>156673991853.39999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2008</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52">
+        <v>1940334</v>
+      </c>
+      <c r="D52">
+        <v>258183027063.90201</v>
+      </c>
+      <c r="E52">
+        <v>272084950947.73999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2013</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <v>238058</v>
+      </c>
+      <c r="D53">
+        <v>10660006571.110001</v>
+      </c>
+      <c r="E53">
+        <v>10660006571.110001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2019</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>1307180</v>
+      </c>
+      <c r="D54">
+        <v>290521335429.48297</v>
+      </c>
+      <c r="E54">
+        <v>290521335195.59003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2023</v>
+      </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>1825</v>
+      </c>
+      <c r="D55">
+        <v>2426093388.1199002</v>
+      </c>
+      <c r="E55">
+        <v>2425955277.3000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1989</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56">
+        <v>2813</v>
+      </c>
+      <c r="D56">
+        <v>1636683946</v>
+      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1995</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>239997</v>
+      </c>
+      <c r="D57">
+        <v>118040376008</v>
+      </c>
+      <c r="E57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1999</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>271684</v>
+      </c>
+      <c r="D58">
+        <v>124700768016.39999</v>
+      </c>
+      <c r="E58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2004</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <v>14</v>
+      </c>
+      <c r="D59">
+        <v>1977972.0639</v>
+      </c>
+      <c r="E59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2008</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60">
+        <v>122875</v>
+      </c>
+      <c r="D60">
+        <v>6214060175.3116999</v>
+      </c>
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2009</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>161851</v>
+      </c>
+      <c r="D61">
+        <v>7259456794.8626003</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1962</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62">
+        <v>5696246</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1980</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63">
+        <v>1214</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63">
+        <v>297556850.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1991</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64">
+        <v>1949</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64">
+        <v>1600668398</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1995</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65">
+        <v>4670</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65">
+        <v>3652587545.8699999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2000</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66">
+        <v>26879</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66">
+        <v>298272849.62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2005</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67">
+        <v>55147.88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2023</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2005</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69">
+        <v>1939319</v>
+      </c>
+      <c r="D69">
+        <v>196075245031.125</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2010</v>
+      </c>
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <v>3350079</v>
+      </c>
+      <c r="D70">
+        <v>530618207041.77502</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2016</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>2059620</v>
+      </c>
+      <c r="D71">
+        <v>247856689926.487</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2023</v>
+      </c>
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72">
+        <v>6667077</v>
+      </c>
+      <c r="D72">
+        <v>757169854900.13599</v>
+      </c>
+      <c r="E72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2004</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73">
+        <v>643412</v>
+      </c>
+      <c r="D73">
+        <v>178758400406.14301</v>
+      </c>
+      <c r="E73">
+        <v>178756981809.17999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2010</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74">
+        <v>193686</v>
+      </c>
+      <c r="D74">
+        <v>30709556862.709999</v>
+      </c>
+      <c r="E74">
+        <v>30709556862.709999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>2015</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75">
+        <v>2856429</v>
+      </c>
+      <c r="D75">
+        <v>255471009664.10001</v>
+      </c>
+      <c r="E75">
+        <v>255471009664.10001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2016</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76">
+        <v>2761714</v>
+      </c>
+      <c r="D76">
+        <v>227629021271.14001</v>
+      </c>
+      <c r="E76">
+        <v>227629021271.14001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2020</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77">
+        <v>1272695</v>
+      </c>
+      <c r="D77">
+        <v>335795205672.448</v>
+      </c>
+      <c r="E77">
+        <v>335795205319.23999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1988</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78">
+        <v>57</v>
+      </c>
+      <c r="D78">
+        <v>7652670</v>
+      </c>
+      <c r="E78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1990</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79">
+        <v>217182</v>
+      </c>
+      <c r="D79">
+        <v>120350129405</v>
+      </c>
+      <c r="E79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>1998</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80">
+        <v>259810</v>
+      </c>
+      <c r="D80">
+        <v>118132963568</v>
+      </c>
+      <c r="E80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2001</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81">
+        <v>10</v>
+      </c>
+      <c r="D81">
+        <v>589000</v>
+      </c>
+      <c r="E81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2010</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>185160</v>
+      </c>
+      <c r="D82">
+        <v>28560945072.699001</v>
+      </c>
+      <c r="E82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2014</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83">
+        <v>212959</v>
+      </c>
+      <c r="D83">
+        <v>8903852404.9487</v>
+      </c>
+      <c r="E83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2017</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84">
+        <v>707262</v>
+      </c>
+      <c r="D84">
+        <v>93960144164.725204</v>
+      </c>
+      <c r="E84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>1967</v>
+      </c>
+      <c r="B85" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85">
+        <v>15397</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>1973</v>
+      </c>
+      <c r="B86" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86">
+        <v>91809</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1977</v>
+      </c>
+      <c r="B87" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>1979</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88">
+        <v>912</v>
+      </c>
+      <c r="D88" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88">
+        <v>4405995486.3100004</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1988</v>
+      </c>
+      <c r="B89" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89">
+        <v>1862</v>
+      </c>
+      <c r="D89" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89">
+        <v>3058722103</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>1989</v>
+      </c>
+      <c r="B90" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90">
+        <v>1518</v>
+      </c>
+      <c r="D90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90">
+        <v>3614072753</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1990</v>
+      </c>
+      <c r="B91" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91">
+        <v>1706</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91">
+        <v>2710272377.25</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1999</v>
+      </c>
+      <c r="B92" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92">
+        <v>89245</v>
+      </c>
+      <c r="D92" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92">
+        <v>40535884551.82</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2001</v>
+      </c>
+      <c r="B93" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93">
+        <v>10</v>
+      </c>
+      <c r="D93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93">
+        <v>2704285.22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>2003</v>
+      </c>
+      <c r="B94" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94">
+        <v>11</v>
+      </c>
+      <c r="D94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94">
+        <v>697600</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2021</v>
+      </c>
+      <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95">
+        <v>52018</v>
+      </c>
+      <c r="D95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95">
+        <v>15853534875.950001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>2007</v>
+      </c>
+      <c r="B96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96">
+        <v>2365738</v>
+      </c>
+      <c r="D96">
+        <v>236463604020.34399</v>
+      </c>
+      <c r="E96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>2015</v>
+      </c>
+      <c r="B97" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97">
+        <v>1518592</v>
+      </c>
+      <c r="D97">
+        <v>184321346847.46301</v>
+      </c>
+      <c r="E97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2019</v>
+      </c>
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98">
+        <v>5182397</v>
+      </c>
+      <c r="D98">
+        <v>300238067280.841</v>
+      </c>
+      <c r="E98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2024</v>
+      </c>
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99">
+        <v>1586095</v>
+      </c>
+      <c r="D99">
+        <v>144392711927.34601</v>
+      </c>
+      <c r="E99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2001</v>
+      </c>
+      <c r="B100" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100">
+        <v>230328</v>
+      </c>
+      <c r="D100">
+        <v>134222343228.45399</v>
+      </c>
+      <c r="E100">
+        <v>134230472446.53999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>2005</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101">
+        <v>984563</v>
+      </c>
+      <c r="D101">
+        <v>195085703055.67401</v>
+      </c>
+      <c r="E101">
+        <v>195085351734.26999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>1992</v>
+      </c>
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102">
+        <v>240574</v>
+      </c>
+      <c r="D102">
+        <v>123406660550</v>
+      </c>
+      <c r="E102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1996</v>
+      </c>
+      <c r="B103" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103">
+        <v>260836</v>
+      </c>
+      <c r="D103">
+        <v>119666794871</v>
+      </c>
+      <c r="E103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>2000</v>
+      </c>
+      <c r="B104" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104">
+        <v>26900</v>
+      </c>
+      <c r="D104">
+        <v>1652230442.4354</v>
+      </c>
+      <c r="E104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>2005</v>
+      </c>
+      <c r="B105" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105">
+        <v>7</v>
+      </c>
+      <c r="D105">
+        <v>55744.080499999996</v>
+      </c>
+      <c r="E105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>2006</v>
+      </c>
+      <c r="B106" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106">
+        <v>4</v>
+      </c>
+      <c r="D106">
+        <v>1542.89</v>
+      </c>
+      <c r="E106" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>2012</v>
+      </c>
+      <c r="B107" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107">
+        <v>196335</v>
+      </c>
+      <c r="D107">
+        <v>8665560052.6476994</v>
+      </c>
+      <c r="E107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2013</v>
+      </c>
+      <c r="B108" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108">
+        <v>215513</v>
+      </c>
+      <c r="D108">
+        <v>8022519483.8234997</v>
+      </c>
+      <c r="E108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>2016</v>
+      </c>
+      <c r="B109" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109">
+        <v>2764158</v>
+      </c>
+      <c r="D109">
+        <v>228728927819.09601</v>
+      </c>
+      <c r="E109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1966</v>
+      </c>
+      <c r="B110" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110">
+        <v>3</v>
+      </c>
+      <c r="D110" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>1974</v>
+      </c>
+      <c r="B111" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111">
+        <v>3</v>
+      </c>
+      <c r="D111" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111">
+        <v>47557300</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1983</v>
+      </c>
+      <c r="B112" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112">
+        <v>1648</v>
+      </c>
+      <c r="D112" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112">
+        <v>1197340749.1500001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>1984</v>
+      </c>
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113">
+        <v>1924</v>
+      </c>
+      <c r="D113" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113">
+        <v>1181650120</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>1987</v>
+      </c>
+      <c r="B114" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114">
+        <v>2559</v>
+      </c>
+      <c r="D114" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114">
+        <v>4113977529</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>1992</v>
+      </c>
+      <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115">
+        <v>2400</v>
+      </c>
+      <c r="D115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115">
+        <v>2566210274</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>1994</v>
+      </c>
+      <c r="B116" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116">
+        <v>2992</v>
+      </c>
+      <c r="D116" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116">
+        <v>16716838097.27</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>1998</v>
+      </c>
+      <c r="B117" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117">
+        <v>56879</v>
+      </c>
+      <c r="D117" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117">
+        <v>30500791029.419998</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>2004</v>
+      </c>
+      <c r="B118" t="s">
+        <v>9</v>
+      </c>
+      <c r="C118">
+        <v>14</v>
+      </c>
+      <c r="D118" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118">
+        <v>2016264.94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>